<commit_message>
plotting milk feeding data
</commit_message>
<xml_diff>
--- a/milk_feeding/data/milk-feeding-practice-among-children-aged-below-2-years-old.xlsx
+++ b/milk_feeding/data/milk-feeding-practice-among-children-aged-below-2-years-old.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamad Aznuddin\Desktop\Data Terbuka\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haoran\Documents\visualising_open_data_malaysia\milk_feeding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF72D62A-2170-41CE-ACE8-8BCA8EA420B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA8EB010-B6D4-4D51-A007-B0F436EEB8F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6910" xr2:uid="{A99EAE0F-AB29-423C-B12E-57631656A288}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A99EAE0F-AB29-423C-B12E-57631656A288}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 19 Milk feeding pratice" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Table 19 Milk feeding pratice'!$1:$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -114,9 +115,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -222,7 +223,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
@@ -230,10 +231,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,21 +243,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -265,38 +278,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1969,25 +1970,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
     </row>
     <row r="2" spans="1:17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1995,52 +1996,52 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="16" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="19" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="22" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
     </row>
     <row r="4" spans="1:17" s="5" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="17" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="17"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="20" t="s">
         <v>0</v>
       </c>
@@ -2049,940 +2050,943 @@
         <v>1</v>
       </c>
       <c r="M4" s="20"/>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23" t="s">
+      <c r="O4" s="14"/>
+      <c r="P4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="23"/>
+      <c r="Q4" s="14"/>
     </row>
     <row r="5" spans="1:17" s="5" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="O5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="Q5" s="22" t="s">
+      <c r="Q5" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="22"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>913788.12411712261</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>88.333867173170404</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>120682.74573138692</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>11.666132826829628</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>419525.92527974083</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>45.93374572117289</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>493802.43210342422</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>54.066254278828872</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>132694.31573351915</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <v>12.835092844590399</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="8">
         <v>901145.62091677077</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <v>87.164907155409693</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="8">
         <v>11735.298010533248</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <v>1.1367364089792606</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P7" s="8">
         <v>1020632.269161088</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="Q7" s="9">
         <v>98.863263591020711</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>108440.71165213706</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>93.645483480998863</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>7358.4786784251446</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>6.3545165190011383</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>69829.373863999717</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>64.394057176609806</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>38611.337788137076</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>35.605942823389938</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="8">
         <v>10418.529520592034</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>9.0064898383935592</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="8">
         <v>105259.49496547494</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <v>90.993510161606466</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="8">
         <v>1673.4184534930873</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <v>1.4451037599797723</v>
       </c>
-      <c r="P8" s="9">
+      <c r="P8" s="8">
         <v>114125.77187706914</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="9">
         <v>98.554896240020241</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>75036.369876244265</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>94.472524722050807</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>4390.2889295937202</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>5.5274752779491534</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>30439.475129092087</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>40.588709643927793</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>44555.456703253069</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <v>59.411290356072421</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <v>16220.431889848744</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="9">
         <v>20.465206232893948</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <v>63038.148284034185</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="9">
         <v>79.534793767106009</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="8">
         <v>471.24817540779026</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="9">
         <v>0.59478348475772946</v>
       </c>
-      <c r="P9" s="9">
+      <c r="P9" s="8">
         <v>78758.957014257438</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="9">
         <v>99.405216515242273</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>65378.873675860254</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>89.723322308097281</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>7488.3273974106251</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>10.276677691902563</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>25783.773155847117</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>39.515033408975683</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>39466.768047011559</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <v>60.484966591024062</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <v>6834.1894827648557</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <v>9.3915875157789817</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="8">
         <v>65935.078452848742</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <v>90.60841248422085</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="8">
         <v>969.6089040259933</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9">
         <v>1.3348453605363368</v>
       </c>
-      <c r="P10" s="9">
+      <c r="P10" s="8">
         <v>71668.685589982488</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="9">
         <v>98.665154639463694</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>27507.026651853063</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>95.405646711454608</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>1324.6280771856214</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>4.5943532885453182</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>10633.722932498998</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>38.678536780352609</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>16858.844826425549</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <v>61.321463219647342</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>3733.3020536154595</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <v>12.948622230327098</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="8">
         <v>25098.352675423223</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <v>87.051377769672825</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="8">
         <v>70.469030709128063</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <v>0.24492533400161728</v>
       </c>
-      <c r="P11" s="9">
+      <c r="P11" s="8">
         <v>28701.169067235751</v>
       </c>
-      <c r="Q11" s="10">
+      <c r="Q11" s="9">
         <v>99.755074665998379</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>37100.901569454392</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>97.798585612471086</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>835.12924030341117</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>2.2014143875289176</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>18587.147170315875</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>50.140626891271999</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>18482.886298993068</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>49.859373108727873</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <v>1201.5358046532995</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>3.1679320675891289</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="8">
         <v>36726.544060004147</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="9">
         <v>96.832067932410808</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="8">
         <v>238.18600503474781</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="9">
         <v>0.6285997913670055</v>
       </c>
-      <c r="P12" s="9">
+      <c r="P12" s="8">
         <v>37653.332303739859</v>
       </c>
-      <c r="Q12" s="10">
+      <c r="Q12" s="9">
         <v>99.37140020863302</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>52419.179718082451</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>81.077816293511475</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>12233.745230363027</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>18.922183706488568</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>17345.056539973881</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>33.089141480767111</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>35074.123178108588</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>66.910858519232917</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <v>9047.7714495874407</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>13.99437296425827</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="8">
         <v>55605.153498858061</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="9">
         <v>86.00562703574181</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="8">
         <v>249.99912235934025</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
         <v>0.38667875051080941</v>
       </c>
-      <c r="P13" s="9">
+      <c r="P13" s="8">
         <v>64402.925826086095</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="Q13" s="9">
         <v>99.613321249489175</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>43289.668455337589</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>96.527638499592001</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>1557.2470273410627</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>3.4723615004080339</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>17444.374633182273</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>40.296854320286194</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>25845.293822155327</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <v>59.703145679713835</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <v>2877.2691849439657</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <v>6.4244745400186156</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="8">
         <v>41908.793348594081</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="9">
         <v>93.575525459981463</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="8">
         <v>989.64786082502769</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <v>2.2082999918973103</v>
       </c>
-      <c r="P14" s="9">
+      <c r="P14" s="8">
         <v>43825.271509561338</v>
       </c>
-      <c r="Q14" s="10">
+      <c r="Q14" s="9">
         <v>97.791700008102751</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>64370.656149466668</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>85.642557170001169</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>10791.340732165878</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>14.357442829998801</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>30876.445908397396</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>48.086963447867163</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>33333.152066886949</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="9">
         <v>51.913036552132965</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <v>21605.357021463566</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="9">
         <v>28.760086185393124</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="8">
         <v>53517.356040629646</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="9">
         <v>71.239913814606965</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="8">
         <v>1581.897874340448</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="9">
         <v>2.106702428300574</v>
       </c>
-      <c r="P15" s="9">
+      <c r="P15" s="8">
         <v>73506.916430417637</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="9">
         <v>97.893297571699392</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>8979.3272047353476</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>91.131137774950801</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>873.86614275679256</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>8.8688622250492148</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>4832.0224310323465</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="9">
         <v>53.861136272624158</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <v>4139.2373035832225</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="9">
         <v>46.138863727375949</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="8">
         <v>1510.2329256134553</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="9">
         <v>15.362604093386526</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="8">
         <v>8320.3460337414763</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="9">
         <v>84.637395906613463</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="8">
         <v>76.287579876737055</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="9">
         <v>0.77640958574396457</v>
       </c>
-      <c r="P16" s="9">
+      <c r="P16" s="8">
         <v>9749.3999538027219</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="Q16" s="9">
         <v>99.223590414256037</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>156978.30623001509</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>84.009292785753559</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>29879.95792696625</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>15.990707214246545</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>67421.697236889842</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <v>42.969365598101099</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <v>89484.732025983001</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>57.030634401898716</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <v>14828.516243974555</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="9">
         <v>7.9383405007095575</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="8">
         <v>171967.65661670253</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="9">
         <v>92.061659499290499</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="8">
         <v>1583.0562244458265</v>
       </c>
-      <c r="O17" s="10">
+      <c r="O17" s="9">
         <v>0.85300206835292902</v>
       </c>
-      <c r="P17" s="9">
+      <c r="P17" s="8">
         <v>184003.38994942658</v>
       </c>
-      <c r="Q17" s="10">
+      <c r="Q17" s="9">
         <v>99.146997931647093</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>36760.949974105766</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>70.241113086212863</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>15574.425077519938</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>29.758886913787897</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>20732.157776669912</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <v>56.397230733355755</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>16028.792197435812</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="9">
         <v>43.602769266644131</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <v>3263.4525968536432</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <v>6.2356534058167501</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="8">
         <v>49071.922454771702</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="9">
         <v>93.764346594183323</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="8">
         <v>64.005868050678302</v>
       </c>
-      <c r="O18" s="10">
+      <c r="O18" s="9">
         <v>0.12229943510969558</v>
       </c>
-      <c r="P18" s="9">
+      <c r="P18" s="8">
         <v>52271.369183574629</v>
       </c>
-      <c r="Q18" s="10">
+      <c r="Q18" s="9">
         <v>99.877700564890304</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>113497.49504071211</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>91.891953262684893</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>10014.402368046936</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>8.1080467373151652</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>53707.623303796965</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="9">
         <v>47.320536267810823</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>59789.871736914843</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="9">
         <v>52.679463732188914</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <v>23460.232583750236</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <v>18.994309921504396</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="8">
         <v>100051.66482500873</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="9">
         <v>81.00569007849559</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="8">
         <v>2269.2183443943964</v>
       </c>
-      <c r="O19" s="10">
+      <c r="O19" s="9">
         <v>1.8385320711966773</v>
       </c>
-      <c r="P19" s="9">
+      <c r="P19" s="8">
         <v>121156.33293888511</v>
       </c>
-      <c r="Q19" s="10">
+      <c r="Q19" s="9">
         <v>98.161467928803305</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>76872.688975027719</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>89.786728634861873</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>8744.2948975533764</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>10.213271365138288</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>33417.806631284395</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <v>43.471624418056003</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>43454.882343743571</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <v>56.528375581944324</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <v>14999.784589704988</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>17.527789828097575</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <v>70577.374520566416</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <v>82.472210171902688</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20" s="8">
         <v>1247.8541290912078</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="9">
         <v>1.4587614592470908</v>
       </c>
-      <c r="P20" s="9">
+      <c r="P20" s="8">
         <v>84294.173402624729</v>
       </c>
-      <c r="Q20" s="10">
+      <c r="Q20" s="9">
         <v>98.541238540752886</v>
       </c>
     </row>
     <row r="21" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>41578.767737701608</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>81.561730388745076</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>9399.5128106956545</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>18.438269611255507</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>16732.897003181453</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <v>40.243850199554792</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>24845.870734520238</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="9">
         <v>59.756149800445399</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="8">
         <v>1765.0195221466106</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="9">
         <v>3.46229708644442</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="8">
         <v>49213.261026250431</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="9">
         <v>96.537702913555734</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N21" s="8">
         <v>205.16281457263045</v>
       </c>
-      <c r="O21" s="10">
+      <c r="O21" s="9">
         <v>0.40245142120447985</v>
       </c>
-      <c r="P21" s="9">
+      <c r="P21" s="8">
         <v>50773.117733824343</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="Q21" s="9">
         <v>99.597548578795539</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="6" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>5577.2012064053524</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>96.253195293973306</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>217.10119505951738</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>3.7468047060269432</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="8">
         <v>1742.3515635751285</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>31.261159937852621</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <v>3831.183030275386</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="9">
         <v>68.738840062148839</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="8">
         <v>928.69086400619221</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="9">
         <v>16.058522756271628</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="8">
         <v>4854.474113877608</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="9">
         <v>83.941477243729338</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N22" s="8">
         <v>45.237623906205712</v>
       </c>
-      <c r="O22" s="10">
+      <c r="O22" s="9">
         <v>0.78175248027375266</v>
       </c>
-      <c r="P22" s="9">
+      <c r="P22" s="8">
         <v>5741.4563806161095</v>
       </c>
-      <c r="Q22" s="10">
+      <c r="Q22" s="9">
         <v>99.218247519726305</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N3:Q3"/>
+  <mergeCells count="30">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="B4:C4"/>
@@ -2999,16 +3003,12 @@
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N3:Q3"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.51181102362204722" top="0.70866141732283472" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="portrait" r:id="rId1"/>

</xml_diff>